<commit_message>
mathstat idz2, algos tasks a,b codeforces
</commit_message>
<xml_diff>
--- a/2COURSE/1SEM/TeorVer/IDZ19.1_var13.xlsx
+++ b/2COURSE/1SEM/TeorVer/IDZ19.1_var13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graev\OneDrive\Рабочий стол\ITMO\2COURSE\1SEM\TeorVer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02FCA6F-58DE-47FB-BEDE-B4FE885F363E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E999DE9-9F6B-4FCE-A50D-A25CD24BB08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4275" windowWidth="16440" windowHeight="28320" xr2:uid="{EB49B44D-FC25-4B73-8993-B04A378E3098}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16656" xr2:uid="{EB49B44D-FC25-4B73-8993-B04A378E3098}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -3391,15 +3391,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>549965</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>148402</xdr:rowOff>
+      <xdr:colOff>146552</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>121507</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>245165</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>108646</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>451352</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>81750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3727,7 +3727,7 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:Y90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Y52" sqref="Y52"/>
     </sheetView>
   </sheetViews>

</xml_diff>